<commit_message>
Added clarification I am capturing from a delta max 2000 battery for commands
</commit_message>
<xml_diff>
--- a/cloud-mqtt/testing_dumps/Key-Value Analysis.xlsx
+++ b/cloud-mqtt/testing_dumps/Key-Value Analysis.xlsx
@@ -1505,8 +1505,8 @@
   <dimension ref="A1:G207"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A27" sqref="A27"/>
+      <pane ySplit="1" topLeftCell="A200" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A208" sqref="A208"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Continuing work on excel sheet
</commit_message>
<xml_diff>
--- a/cloud-mqtt/testing_dumps/Key-Value Analysis.xlsx
+++ b/cloud-mqtt/testing_dumps/Key-Value Analysis.xlsx
@@ -1505,8 +1505,8 @@
   <dimension ref="A1:G207"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A200" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A208" sqref="A208"/>
+      <pane ySplit="1" topLeftCell="A36" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A55" sqref="A55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Fixed mapping in excel Added more detail in get-login Added home-assistant sensor package Added example lovelace
</commit_message>
<xml_diff>
--- a/cloud-mqtt/testing_dumps/Key-Value Analysis.xlsx
+++ b/cloud-mqtt/testing_dumps/Key-Value Analysis.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="552" uniqueCount="367">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="559" uniqueCount="367">
   <si>
     <t>bmsMaster.amp</t>
   </si>
@@ -1107,9 +1107,6 @@
     <t>Discharge</t>
   </si>
   <si>
-    <t>Missing/Unknown</t>
-  </si>
-  <si>
     <t>Car Input Max Amps</t>
   </si>
   <si>
@@ -1120,6 +1117,9 @@
   </si>
   <si>
     <t>Minutes</t>
+  </si>
+  <si>
+    <t>** None, appears to be polled by sending 'set' command "params": {"id": 72} and monitoring set_reply for "data": {"data": 8000,"cmdSet": 32,"ack": 0,"id": 72} the "data" value of 8000 is 8 Amps</t>
   </si>
 </sst>
 </file>
@@ -1191,7 +1191,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -1201,6 +1201,10 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1502,16 +1506,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G207"/>
+  <dimension ref="A1:G208"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A36" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A55" sqref="A55"/>
+      <pane ySplit="1" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B66" sqref="B66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.25" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.625" customWidth="1"/>
     <col min="2" max="2" width="55.5" customWidth="1"/>
     <col min="3" max="3" width="10.75" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.75" bestFit="1" customWidth="1"/>
@@ -2106,7 +2110,7 @@
       <c r="A37" t="s">
         <v>35</v>
       </c>
-      <c r="B37" s="2" t="s">
+      <c r="B37" s="7" t="s">
         <v>302</v>
       </c>
       <c r="C37" t="s">
@@ -2114,6 +2118,9 @@
       </c>
       <c r="D37" t="s">
         <v>265</v>
+      </c>
+      <c r="E37" t="s">
+        <v>349</v>
       </c>
       <c r="F37" s="1" t="s">
         <v>236</v>
@@ -2163,7 +2170,7 @@
       <c r="A41" t="s">
         <v>39</v>
       </c>
-      <c r="B41" s="2" t="s">
+      <c r="B41" s="7" t="s">
         <v>303</v>
       </c>
       <c r="C41" t="s">
@@ -2171,6 +2178,9 @@
       </c>
       <c r="D41" t="s">
         <v>265</v>
+      </c>
+      <c r="E41" t="s">
+        <v>349</v>
       </c>
       <c r="F41">
         <v>5999</v>
@@ -2778,6 +2788,18 @@
       <c r="A75" t="s">
         <v>73</v>
       </c>
+      <c r="B75" s="7" t="s">
+        <v>283</v>
+      </c>
+      <c r="C75" t="s">
+        <v>249</v>
+      </c>
+      <c r="D75" t="s">
+        <v>249</v>
+      </c>
+      <c r="E75" t="s">
+        <v>349</v>
+      </c>
       <c r="F75">
         <v>0</v>
       </c>
@@ -2940,11 +2962,14 @@
       <c r="A84" t="s">
         <v>82</v>
       </c>
-      <c r="B84" t="s">
+      <c r="B84" s="7" t="s">
         <v>263</v>
       </c>
       <c r="D84" t="s">
         <v>265</v>
+      </c>
+      <c r="E84" t="s">
+        <v>349</v>
       </c>
       <c r="F84" s="1" t="s">
         <v>264</v>
@@ -3753,18 +3778,6 @@
       <c r="A141" t="s">
         <v>139</v>
       </c>
-      <c r="B141" s="7" t="s">
-        <v>283</v>
-      </c>
-      <c r="C141" t="s">
-        <v>249</v>
-      </c>
-      <c r="D141" t="s">
-        <v>249</v>
-      </c>
-      <c r="E141" t="s">
-        <v>349</v>
-      </c>
       <c r="F141" s="1" t="s">
         <v>255</v>
       </c>
@@ -4229,7 +4242,7 @@
         <v>180</v>
       </c>
       <c r="B182" s="8" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="C182" t="s">
         <v>285</v>
@@ -4322,7 +4335,7 @@
       <c r="A187" t="s">
         <v>185</v>
       </c>
-      <c r="B187" s="2" t="s">
+      <c r="B187" s="7" t="s">
         <v>289</v>
       </c>
       <c r="C187" t="s">
@@ -4330,6 +4343,9 @@
       </c>
       <c r="D187" t="s">
         <v>265</v>
+      </c>
+      <c r="E187" t="s">
+        <v>349</v>
       </c>
       <c r="F187" s="1" t="s">
         <v>290</v>
@@ -4363,10 +4379,10 @@
         <v>187</v>
       </c>
       <c r="B189" s="8" t="s">
+        <v>364</v>
+      </c>
+      <c r="C189" t="s">
         <v>365</v>
-      </c>
-      <c r="C189" t="s">
-        <v>366</v>
       </c>
       <c r="D189" t="s">
         <v>265</v>
@@ -4661,13 +4677,31 @@
         <v>0</v>
       </c>
     </row>
-    <row r="207" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A207" t="s">
+    <row r="207" spans="1:7" ht="120" x14ac:dyDescent="0.25">
+      <c r="A207" s="9" t="s">
+        <v>366</v>
+      </c>
+      <c r="B207" s="8" t="s">
         <v>362</v>
       </c>
-      <c r="B207" t="s">
-        <v>363</v>
-      </c>
+      <c r="C207" t="s">
+        <v>208</v>
+      </c>
+      <c r="D207" t="s">
+        <v>220</v>
+      </c>
+      <c r="E207" t="s">
+        <v>358</v>
+      </c>
+      <c r="F207">
+        <v>8000</v>
+      </c>
+      <c r="G207">
+        <v>8000</v>
+      </c>
+    </row>
+    <row r="208" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A208" s="10"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:G207"/>

</xml_diff>